<commit_message>
[DataTable] ConfigTable 구조 추가
</commit_message>
<xml_diff>
--- a/DataTable/FarmerSalesTable.xlsx
+++ b/DataTable/FarmerSalesTable.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\ProjectF\DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seh00n/GitHub/ProjectF/DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25BEF2B9-AE0C-42C2-AE8F-704A55C8D7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05D9A73-A422-4447-B65F-CE4B21A0E231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FA5AC356-2F7D-4E04-A31B-16325DD2973F}"/>
+    <workbookView xWindow="2120" yWindow="-16680" windowWidth="29040" windowHeight="15720" xr2:uid="{FA5AC356-2F7D-4E04-A31B-16325DD2973F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FarmerSalesTable" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>id</t>
   </si>
@@ -62,12 +62,16 @@
     <t>1.6f</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,21 +653,21 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="25.125" customWidth="1"/>
-    <col min="4" max="4" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18" thickBot="1">
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +679,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="18" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -687,7 +691,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="18" thickBot="1">
       <c r="A4" s="5">
         <v>0</v>
       </c>

</xml_diff>